<commit_message>
Create Schema + ETL Tools
</commit_message>
<xml_diff>
--- a/xls/template.xlsx
+++ b/xls/template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\uni\econostat\lal\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\uni\econostat\my-contribs\database\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04F0CCC-129B-4E22-9BE9-3AFB8CF4D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E7240C-520A-42B1-8CB6-6162AA847D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="2880" windowWidth="15870" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="2775" windowWidth="15870" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="default" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -668,9 +668,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,10 +687,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -958,13 +955,18 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="2">
+        <v>44500</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>